<commit_message>
Adds more methods for loading/storing datasets. Adds one more activation function. Adds more configuration options for a Model.
</commit_message>
<xml_diff>
--- a/src/test/resources/test_model.xlsx
+++ b/src/test/resources/test_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\build\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7739BD6-32D2-4BC1-A6A1-947460B2803F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6AE91-8CD2-41F0-B224-B1E1A12C120E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Learning Factor" sheetId="1" r:id="rId1"/>
@@ -379,15 +379,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -438,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>

</xml_diff>